<commit_message>
apply hungarian algorithm for visualization
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010"/>
+    <workbookView windowWidth="19815" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -43,6 +43,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>batch size =</t>
     </r>
     <r>
@@ -74,6 +81,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>epoch = 800/</t>
     </r>
     <r>
@@ -99,6 +113,30 @@
   <si>
     <t>ImageNet(supervised,basic pretrained resnet for classification)</t>
   </si>
+  <si>
+    <t>factorization</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>reconstruction error</t>
+  </si>
+  <si>
+    <t>norm(hyperfeat)</t>
+  </si>
+  <si>
+    <t>error/norm</t>
+  </si>
+  <si>
+    <t>Kmeans</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>NMF</t>
+  </si>
 </sst>
 </file>
 
@@ -110,14 +148,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,48 +613,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -633,97 +667,94 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1087,7 +1118,7 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1205,14 +1236,92 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="12.625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>218.13</v>
+      </c>
+      <c r="D2">
+        <v>333.15</v>
+      </c>
+      <c r="E2">
+        <f>C2/D2</f>
+        <v>0.654750112561909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>287.40118</v>
+      </c>
+      <c r="D3">
+        <v>333.15</v>
+      </c>
+      <c r="E3">
+        <f>C3/D3</f>
+        <v>0.862678012907099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>151.40488</v>
+      </c>
+      <c r="D4">
+        <v>261.87</v>
+      </c>
+      <c r="E4">
+        <f>C4/D4</f>
+        <v>0.578168098674915</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
change model load and move the project to bianca
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" activeTab="1"/>
+    <workbookView windowWidth="19815" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>variation</t>
+  </si>
+  <si>
+    <t>PCK</t>
   </si>
   <si>
     <t>simsiam</t>
@@ -114,7 +117,10 @@
     <t>ImageNet(supervised,basic pretrained resnet for classification)</t>
   </si>
   <si>
-    <t>factorization</t>
+    <t>factorization(applied after Relu)</t>
+  </si>
+  <si>
+    <t>backbone</t>
   </si>
   <si>
     <t>k</t>
@@ -130,6 +136,9 @@
   </si>
   <si>
     <t>Kmeans</t>
+  </si>
+  <si>
+    <t>resnet50_densecl_IN</t>
   </si>
   <si>
     <t>PCA</t>
@@ -142,16 +151,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -616,10 +632,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -628,34 +644,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -667,105 +680,120 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,13 +1144,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="9.875" customWidth="1"/>
     <col min="3" max="3" width="63.375" customWidth="1"/>
@@ -1130,14 +1158,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1150,77 +1178,92 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.354</v>
       </c>
     </row>
   </sheetData>
@@ -1236,89 +1279,354 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
-    <col min="5" max="5" width="12.625"/>
+    <col min="1" max="1" width="38.125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
+    <col min="6" max="6" width="12.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>134.91</v>
+      </c>
+      <c r="E2">
+        <v>238.41</v>
+      </c>
+      <c r="F2">
+        <f>D2/E2</f>
+        <v>0.565873914684787</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>211.39</v>
+      </c>
+      <c r="E3">
+        <v>238.41</v>
+      </c>
+      <c r="F3">
+        <f>D3/E3</f>
+        <v>0.88666582777568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>127.02</v>
+      </c>
+      <c r="E4">
+        <v>238.41</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F16" si="0">D4/E4</f>
+        <v>0.532779665282497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>121.86</v>
+      </c>
+      <c r="E5">
+        <v>238.41</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.511136277840695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>202.07</v>
+      </c>
+      <c r="E6">
+        <v>238.41</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.847573507822658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>110.07</v>
+      </c>
+      <c r="E7">
+        <v>238.41</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.461683654209135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>218.13</v>
-      </c>
-      <c r="D2">
-        <v>333.15</v>
-      </c>
-      <c r="E2">
-        <f>C2/D2</f>
-        <v>0.654750112561909</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>287.40118</v>
-      </c>
-      <c r="D3">
-        <v>333.15</v>
-      </c>
-      <c r="E3">
-        <f>C3/D3</f>
-        <v>0.862678012907099</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="D8">
+        <v>111.25</v>
+      </c>
+      <c r="E8">
+        <v>238.41</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.466633111027222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>195</v>
+      </c>
+      <c r="E9">
+        <v>238.41</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.817918711463445</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>96.32</v>
+      </c>
+      <c r="E10">
+        <v>238.41</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.404009898913636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>151.40488</v>
-      </c>
-      <c r="D4">
-        <v>261.87</v>
-      </c>
-      <c r="E4">
-        <f>C4/D4</f>
-        <v>0.578168098674915</v>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>103.2</v>
+      </c>
+      <c r="E11">
+        <v>238.41</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.432867748836039</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>189.53</v>
+      </c>
+      <c r="E12">
+        <v>238.41</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.794975042993163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>85.58</v>
+      </c>
+      <c r="E13">
+        <v>238.41</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.358961452959188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <v>96.12</v>
+      </c>
+      <c r="E14">
+        <v>238.41</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.40317100792752</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="D15">
+        <v>185.38</v>
+      </c>
+      <c r="E15">
+        <v>238.41</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.777568055031249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1">
+        <v>75.6</v>
+      </c>
+      <c r="E16">
+        <v>238.41</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.317100792751982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding factorize,normalize,relu to experiments
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -30,10 +30,28 @@
     <t>pretrained dataset</t>
   </si>
   <si>
+    <t>hyperfeats_id</t>
+  </si>
+  <si>
     <t>variation</t>
   </si>
   <si>
-    <t>PCK</t>
+    <t>PCK(without factorization)</t>
+  </si>
+  <si>
+    <t>PCK(with factorization)</t>
+  </si>
+  <si>
+    <t>PCK(with mutual normalization)</t>
+  </si>
+  <si>
+    <t>PCk(with mutual normalization and factorization)</t>
+  </si>
+  <si>
+    <t>PCK(with ReLU)</t>
+  </si>
+  <si>
+    <t>PCK(with ReLU and factorization)</t>
   </si>
   <si>
     <t>simsiam</t>
@@ -43,6 +61,9 @@
   </si>
   <si>
     <t>ImageNet(unsupervised,as specified in the paper)</t>
+  </si>
+  <si>
+    <t>(0,11,12,13)</t>
   </si>
   <si>
     <r>
@@ -109,6 +130,9 @@
   </si>
   <si>
     <t>resnet101</t>
+  </si>
+  <si>
+    <t>(0,19,27,28,29,30)</t>
   </si>
   <si>
     <t>SCOT</t>
@@ -774,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -784,17 +808,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1144,131 +1171,215 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="2" max="2" width="9.875" customWidth="1"/>
-    <col min="3" max="3" width="63.375" customWidth="1"/>
-    <col min="4" max="4" width="21.25" customWidth="1"/>
+    <col min="3" max="3" width="31.125" customWidth="1"/>
+    <col min="4" max="5" width="21.25" customWidth="1"/>
+    <col min="6" max="7" width="14.875" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" ht="30" customHeight="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:11">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4">
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:11">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5">
         <v>0.232</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:11">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.233</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:11">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="E5" s="3"/>
+      <c r="F5" s="7">
+        <v>0.237</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:11">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="6">
+        <v>0.217</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:11">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6">
         <v>0.321</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:11">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6">
         <v>0.354</v>
       </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1296,30 +1407,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1337,10 +1448,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1358,10 +1469,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -1379,10 +1490,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1400,10 +1511,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -1421,10 +1532,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1442,10 +1553,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1463,10 +1574,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1484,10 +1595,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1505,10 +1616,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1526,10 +1637,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1547,10 +1658,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>25</v>
@@ -1568,10 +1679,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>36</v>
@@ -1589,10 +1700,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>36</v>
@@ -1610,10 +1721,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>36</v>

</xml_diff>

<commit_message>
change the order of G
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010"/>
+    <workbookView windowWidth="19815" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -141,6 +141,26 @@
     <t>ImageNet(supervised,basic pretrained resnet for classification)</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">pca_k=4:8.6%;kmeans_k=4:9.7%; pca_k=100:16.1%  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pca_k=4(ordered):5.3%;pca_k=100(ordered):5.9%</t>
+    </r>
+  </si>
+  <si>
+    <t>pca_k=100:14.8%</t>
+  </si>
+  <si>
+    <t>pca_k=100:15.5%</t>
+  </si>
+  <si>
     <t>factorization(applied after Relu)</t>
   </si>
   <si>
@@ -198,6 +218,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -338,13 +365,6 @@
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -656,10 +676,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -668,34 +688,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -707,98 +724,101 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -821,6 +841,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1173,8 +1196,8 @@
   <sheetPr/>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
@@ -1182,7 +1205,8 @@
     <col min="2" max="2" width="9.875" customWidth="1"/>
     <col min="3" max="3" width="31.125" customWidth="1"/>
     <col min="4" max="5" width="21.25" customWidth="1"/>
-    <col min="6" max="7" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="27.75" customWidth="1"/>
     <col min="8" max="8" width="16.625" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
@@ -1348,11 +1372,21 @@
       <c r="F7" s="6">
         <v>0.321</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="G7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.309</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.296</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -1372,7 +1406,6 @@
         <v>0.354</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1392,7 +1425,7 @@
   <sheetPr/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1407,30 +1440,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1448,10 +1481,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1469,10 +1502,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -1490,10 +1523,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1511,10 +1544,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -1532,10 +1565,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1553,10 +1586,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1574,10 +1607,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1595,10 +1628,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1616,10 +1649,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1637,10 +1670,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1658,10 +1691,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>25</v>
@@ -1679,10 +1712,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>36</v>
@@ -1700,10 +1733,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>36</v>
@@ -1721,10 +1754,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>36</v>

</xml_diff>

<commit_message>
change pca to svd
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" activeTab="1"/>
+    <workbookView windowWidth="19815" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,23 +142,36 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">pca_k=4:8.6%;kmeans_k=4:9.7%; pca_k=100:16.1%  </t>
+      <t xml:space="preserve">pca_k=4:8.6%;kmeans_k=4:9.7%; pca_k=100:16.1%  pca_k=4(ordered):5.3%;pca_k=100(ordered):5.9% </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>pca_k=4(ordered):5.3%;pca_k=100(ordered):5.9%</t>
+      <t>svd_k=4(ordered):8.6%,svd_k=100(ordered):8.6%</t>
     </r>
   </si>
   <si>
     <t>pca_k=100:14.8%</t>
   </si>
   <si>
-    <t>pca_k=100:15.5%</t>
+    <r>
+      <t>pca_k=100:15.5%,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nmf_k=4(ordered):8.7%</t>
+    </r>
   </si>
   <si>
     <t>factorization(applied after Relu)</t>
@@ -1196,8 +1209,8 @@
   <sheetPr/>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
@@ -1206,7 +1219,7 @@
     <col min="3" max="3" width="31.125" customWidth="1"/>
     <col min="4" max="5" width="21.25" customWidth="1"/>
     <col min="6" max="6" width="14.875" customWidth="1"/>
-    <col min="7" max="7" width="27.75" customWidth="1"/>
+    <col min="7" max="7" width="49.5" customWidth="1"/>
     <col min="8" max="8" width="16.625" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
@@ -1425,7 +1438,7 @@
   <sheetPr/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tried removing RHM, not good
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" activeTab="2"/>
+    <workbookView windowWidth="19815" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="55">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -142,6 +144,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">pca_k=4:8.6%;kmeans_k=4:9.7%; pca_k=100:16.1%  pca_k=4(ordered):5.3%;pca_k=100(ordered):5.9% </t>
     </r>
     <r>
@@ -157,6 +166,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">pca_k=100:14.8% </t>
     </r>
     <r>
@@ -225,7 +241,7 @@
     <t>PCK for SCOT with default resnet50 pretrained on ImageNet(Supervised,for classification) as the backbone</t>
   </si>
   <si>
-    <t>PCK(reconstruction with PCA)</t>
+    <t>PCK(reconstruction with PCA without zero mean(SVD))</t>
   </si>
   <si>
     <t>PCK(reconstruction with Kmeans)</t>
@@ -234,7 +250,7 @@
     <t>PCK(ReLU)</t>
   </si>
   <si>
-    <t>PCK(ReLU+reconstruction with PCA)</t>
+    <t>PCK(ReLU+reconstruction with PCA without zero mean(SVD))</t>
   </si>
   <si>
     <t>PCK(ReLU+reconstruction with KMeans)</t>
@@ -244,6 +260,33 @@
   </si>
   <si>
     <t>32.1%(baseline)</t>
+  </si>
+  <si>
+    <t>32.2%(30.8% with pca with zero mean,31.0% with pca with mutual mean)</t>
+  </si>
+  <si>
+    <t>Different pretrained backbones with corresponding optimal hyperfeats_id</t>
+  </si>
+  <si>
+    <t>PCK</t>
+  </si>
+  <si>
+    <t>(0, 8, 10, 11, 12, 13, 14, 15)</t>
+  </si>
+  <si>
+    <t>(0, 7, 8, 9, 10, 11, 12)</t>
+  </si>
+  <si>
+    <t>Different pretrained backbones without RHM, w/o mutual normalization</t>
+  </si>
+  <si>
+    <t>mutual normalization</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -879,13 +922,22 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -901,19 +953,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1272,8 +1312,8 @@
   <sheetPr/>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
@@ -1290,201 +1330,201 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:7">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:11">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:11">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="10">
         <v>0.232</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:11">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="6">
         <v>0.233</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:11">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="12">
+      <c r="E5" s="2"/>
+      <c r="F5" s="11">
         <v>0.237</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:11">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="11">
+      <c r="E6" s="2"/>
+      <c r="F6" s="6">
         <v>0.217</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:11">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="11">
+      <c r="E7" s="2"/>
+      <c r="F7" s="6">
         <v>0.321</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="6">
         <v>0.309</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="6">
         <v>0.296</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:11">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="11">
+      <c r="E8" s="2"/>
+      <c r="F8" s="6">
         <v>0.354</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1838,7 +1878,7 @@
       <c r="C16">
         <v>36</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="9">
         <v>75.6</v>
       </c>
       <c r="E16">
@@ -1861,8 +1901,8 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -1870,99 +1910,102 @@
     <col min="1" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A3" s="1">
+    <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="2">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
         <v>0.142</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>0.138</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="7">
         <v>0.296</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>0.126</v>
       </c>
-      <c r="H3" s="3">
+      <c r="G3" s="6">
+        <v>0.142</v>
+      </c>
+      <c r="H3" s="6">
         <v>0.123</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A4" s="1">
+    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A4" s="2">
         <v>100</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="5">
+      <c r="B4" s="5"/>
+      <c r="C4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A5" s="2">
+        <v>200</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="8">
         <v>0.322</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A5" s="1">
-        <v>200</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5">
-        <v>0.322</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A6" s="1">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A6" s="2">
         <v>400</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6">
         <v>0.321</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="30" customHeight="1"/>
-    <row r="8" s="1" customFormat="1" ht="30" customHeight="1"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="30" customHeight="1"/>
+    <row r="8" s="2" customFormat="1" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
@@ -1973,4 +2016,277 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="2" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="19.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.266</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.321</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="2" width="20.625" customWidth="1"/>
+    <col min="3" max="3" width="26.125" customWidth="1"/>
+    <col min="4" max="6" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="35" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" ht="35" customHeight="1" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" ht="35" customHeight="1" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" ht="35" customHeight="1" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" ht="35" customHeight="1" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" ht="35" customHeight="1" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="7" ht="35" customHeight="1" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.305</v>
+      </c>
+    </row>
+    <row r="8" ht="35" customHeight="1" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.287</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add clip and move to sinergia
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" activeTab="4"/>
+    <workbookView windowWidth="19815" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>ImageNet(self-supervised,as specified in the paper)</t>
+  </si>
+  <si>
+    <t>clip</t>
   </si>
   <si>
     <t>resnet101</t>
@@ -466,7 +469,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +479,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -780,10 +789,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -792,16 +801,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -813,10 +822,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -837,28 +846,28 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -867,19 +876,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -891,38 +897,41 @@
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -950,11 +959,20 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1310,13 +1328,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="9.875" customWidth="1"/>
     <col min="3" max="3" width="31.125" customWidth="1"/>
@@ -1391,7 +1409,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>0.232</v>
       </c>
       <c r="G3" s="2"/>
@@ -1439,7 +1457,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="11">
+      <c r="F5" s="14">
         <v>0.237</v>
       </c>
       <c r="G5" s="2"/>
@@ -1450,20 +1468,18 @@
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:11">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="E6" s="12"/>
       <c r="F6" s="6">
-        <v>0.217</v>
+        <v>0.21</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1473,58 +1489,81 @@
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:11">
       <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="6">
-        <v>0.321</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0.309</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0.296</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>27</v>
-      </c>
+        <v>0.217</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="6">
+        <v>0.321</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.309</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.296</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:11">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6">
         <v>0.354</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1556,30 +1595,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1597,10 +1636,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1618,10 +1657,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -1639,10 +1678,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1660,10 +1699,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -1681,10 +1720,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1702,10 +1741,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1723,10 +1762,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1744,10 +1783,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1765,10 +1804,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1786,10 +1825,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1807,10 +1846,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>25</v>
@@ -1828,10 +1867,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>36</v>
@@ -1849,10 +1888,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
       </c>
       <c r="C15">
         <v>36</v>
@@ -1870,15 +1909,15 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>36</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="13">
         <v>75.6</v>
       </c>
       <c r="E16">
@@ -1901,8 +1940,8 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -1912,7 +1951,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1924,28 +1963,28 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
@@ -1953,7 +1992,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6">
         <v>0.142</v>
@@ -1974,17 +2013,29 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:5">
+    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A4" s="2">
         <v>100</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.272</v>
       </c>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="F4" s="8">
+        <v>0.298</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.265</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.292</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A5" s="2">
         <v>200</v>
       </c>
@@ -1992,9 +2043,21 @@
       <c r="C5" s="8">
         <v>0.322</v>
       </c>
+      <c r="D5" s="9">
+        <v>0.291</v>
+      </c>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="F5" s="10">
+        <v>0.297</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.276</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.296</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A6" s="2">
         <v>400</v>
       </c>
@@ -2002,10 +2065,34 @@
       <c r="C6" s="6">
         <v>0.321</v>
       </c>
+      <c r="D6" s="11">
+        <v>0.31</v>
+      </c>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" s="2" customFormat="1" ht="30" customHeight="1"/>
-    <row r="8" s="2" customFormat="1" ht="30" customHeight="1"/>
+      <c r="F6" s="9">
+        <v>0.296</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.286</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.295</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A7" s="2">
+        <v>600</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A8" s="2">
+        <v>800</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
@@ -2036,7 +2123,7 @@
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2057,7 +2144,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:5">
@@ -2071,7 +2158,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="4">
         <v>0.266</v>
@@ -2088,7 +2175,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E4" s="4">
         <v>0.27</v>
@@ -2096,13 +2183,13 @@
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -2125,8 +2212,8 @@
   <sheetPr/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="5"/>
@@ -2138,7 +2225,7 @@
   <sheetData>
     <row r="1" ht="35" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2160,10 +2247,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" ht="35" customHeight="1" spans="1:6">
@@ -2177,12 +2264,14 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.248</v>
+      </c>
     </row>
     <row r="4" ht="35" customHeight="1" spans="1:6">
       <c r="A4" s="2" t="s">
@@ -2195,12 +2284,14 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.238</v>
+      </c>
     </row>
     <row r="5" ht="35" customHeight="1" spans="1:6">
       <c r="A5" s="2" t="s">
@@ -2213,10 +2304,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" s="4">
         <v>0.26</v>
@@ -2233,10 +2324,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F6" s="4">
         <v>0.248</v>
@@ -2244,19 +2335,19 @@
     </row>
     <row r="7" ht="35" customHeight="1" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F7" s="4">
         <v>0.305</v>
@@ -2264,19 +2355,19 @@
     </row>
     <row r="8" ht="35" customHeight="1" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F8" s="4">
         <v>0.287</v>

</xml_diff>

<commit_message>
investigate hook func, clip normalize, scratch
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" activeTab="2"/>
+    <workbookView windowWidth="19815" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -134,6 +134,9 @@
     <t>clip</t>
   </si>
   <si>
+    <t>new normalization</t>
+  </si>
+  <si>
     <t>resnet101</t>
   </si>
   <si>
@@ -265,6 +268,9 @@
     <t>32.1%(baseline)</t>
   </si>
   <si>
+    <t>29.6%(baseline)</t>
+  </si>
+  <si>
     <t>32.2%(30.8% with pca with zero mean,31.0% with pca with mutual mean)</t>
   </si>
   <si>
@@ -278,6 +284,15 @@
   </si>
   <si>
     <t>(0, 7, 8, 9, 10, 11, 12)</t>
+  </si>
+  <si>
+    <t>CLIP</t>
+  </si>
+  <si>
+    <t>(0, 4, 10, 12, 13)</t>
+  </si>
+  <si>
+    <t>resnet50(new normalization)</t>
   </si>
   <si>
     <t>Different pretrained backbones without RHM, w/o mutual normalization</t>
@@ -469,7 +484,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,12 +494,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,10 +798,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -801,16 +810,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -822,52 +831,52 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -876,16 +885,19 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -897,41 +909,38 @@
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -965,16 +974,13 @@
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1328,10 +1334,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1457,7 +1463,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>0.237</v>
       </c>
       <c r="G5" s="2"/>
@@ -1477,9 +1483,9 @@
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="6">
-        <v>0.21</v>
+      <c r="E6" s="13"/>
+      <c r="F6" s="8">
+        <v>0.261</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1489,20 +1495,20 @@
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6">
-        <v>0.217</v>
+      <c r="F7" s="8">
+        <v>0.279</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1512,58 +1518,81 @@
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:11">
       <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="6">
-        <v>0.321</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.309</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="6">
-        <v>0.296</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>28</v>
-      </c>
+        <v>0.217</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" ht="30" customHeight="1" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="6">
+        <v>0.321</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.309</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.296</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:11">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="6">
         <v>0.354</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1595,30 +1624,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1636,10 +1665,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1657,10 +1686,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -1678,10 +1707,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1699,10 +1728,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -1720,10 +1749,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -1741,10 +1770,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1762,10 +1791,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1783,10 +1812,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -1804,10 +1833,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1825,10 +1854,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1846,10 +1875,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>25</v>
@@ -1867,10 +1896,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>36</v>
@@ -1888,10 +1917,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
       </c>
       <c r="C15">
         <v>36</v>
@@ -1909,15 +1938,15 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>36</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="11">
         <v>75.6</v>
       </c>
       <c r="E16">
@@ -1940,8 +1969,8 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -1951,7 +1980,7 @@
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1963,28 +1992,28 @@
     </row>
     <row r="2" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
@@ -1992,7 +2021,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6">
         <v>0.142</v>
@@ -2000,8 +2029,8 @@
       <c r="D3" s="6">
         <v>0.138</v>
       </c>
-      <c r="E3" s="7">
-        <v>0.296</v>
+      <c r="E3" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="F3" s="6">
         <v>0.126</v>
@@ -2019,12 +2048,12 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="9">
         <v>0.272</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="8">
         <v>0.298</v>
       </c>
@@ -2046,7 +2075,7 @@
       <c r="D5" s="9">
         <v>0.291</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="10">
         <v>0.297</v>
       </c>
@@ -2065,14 +2094,14 @@
       <c r="C6" s="6">
         <v>0.321</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>0.31</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="9">
         <v>0.296</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>0.286</v>
       </c>
       <c r="H6" s="9">
@@ -2083,21 +2112,33 @@
       <c r="A7" s="2">
         <v>600</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="5"/>
+      <c r="D7" s="9">
+        <v>0.315</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="G7" s="9">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
       <c r="A8" s="2">
         <v>800</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="5"/>
+      <c r="D8" s="9">
+        <v>0.317</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="G8" s="9">
+        <v>0.292</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="E3:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2108,13 +2149,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="15.625" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
@@ -2123,7 +2164,7 @@
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2144,7 +2185,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1" spans="1:5">
@@ -2158,7 +2199,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" s="4">
         <v>0.266</v>
@@ -2175,7 +2216,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4">
         <v>0.27</v>
@@ -2183,13 +2224,13 @@
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
@@ -2198,6 +2239,29 @@
         <v>0.321</v>
       </c>
     </row>
+    <row r="6" ht="30" customHeight="1" spans="1:5">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.266</v>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
@@ -2225,7 +2289,7 @@
   <sheetData>
     <row r="1" ht="35" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2247,10 +2311,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" ht="35" customHeight="1" spans="1:6">
@@ -2264,10 +2328,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F3" s="4">
         <v>0.248</v>
@@ -2284,10 +2348,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F4" s="4">
         <v>0.238</v>
@@ -2304,10 +2368,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F5" s="4">
         <v>0.26</v>
@@ -2324,10 +2388,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F6" s="4">
         <v>0.248</v>
@@ -2335,19 +2399,19 @@
     </row>
     <row r="7" ht="35" customHeight="1" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F7" s="4">
         <v>0.305</v>
@@ -2355,19 +2419,19 @@
     </row>
     <row r="8" ht="35" customHeight="1" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F8" s="4">
         <v>0.287</v>

</xml_diff>

<commit_message>
evaluate on gta and cityscape
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,22 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" activeTab="3"/>
+    <workbookView windowWidth="19815" windowHeight="8010" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="facr on SCOT" sheetId="3" r:id="rId3"/>
+    <sheet name="facr on clip" sheetId="6" r:id="rId4"/>
+    <sheet name="optimal hyperfeats" sheetId="4" r:id="rId5"/>
+    <sheet name="mutual normalization" sheetId="5" r:id="rId6"/>
+    <sheet name="Test on gta" sheetId="7" r:id="rId7"/>
+    <sheet name="Test on gta (fix data)" sheetId="9" r:id="rId8"/>
+    <sheet name="facr on SCOT (gta)" sheetId="10" r:id="rId9"/>
+    <sheet name="gta beamsearch(on test)" sheetId="8" r:id="rId10"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="96">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -315,6 +320,158 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Test results on gta&amp;cityscape datasets of different backbones</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>Normalized Acc</t>
+  </si>
+  <si>
+    <t>Acc(without RHM)</t>
+  </si>
+  <si>
+    <t>Normalized Acc(Without RHM)</t>
+  </si>
+  <si>
+    <t>Acc(without CAM)</t>
+  </si>
+  <si>
+    <t>Normalized Acc(Without CAM)</t>
+  </si>
+  <si>
+    <t>spair normalization(wrong)</t>
+  </si>
+  <si>
+    <t>36.6%?</t>
+  </si>
+  <si>
+    <t>41.0%?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45.0%/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45.2%/46.4%/46.2%/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>47.2%</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50.9%/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>50.7%/51.6%/51.4%/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>52.4%</t>
+    </r>
+  </si>
+  <si>
+    <t>46%/46.0%</t>
+  </si>
+  <si>
+    <t>51.6%/52.1%</t>
+  </si>
+  <si>
+    <t>Test results on gta&amp;cityscape datasets(the first 500 images) of different backbones</t>
+  </si>
+  <si>
+    <t>gta denormalization</t>
+  </si>
+  <si>
+    <t>PCK for SCOT with default resnet50 pretrained on ImageNet(Supervised,for classification) as the backbone(hyperfeature_id = 0, 2, 9, 13),without CAM</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(without factorization)</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(reconstruction with SVD)</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(reconstruction with Kmeans)</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(ReLU)</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(ReLU+reconstruction with SVD)</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(ReLU+reconstruction with KMeans)</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(ReLU+reconstruction with NMF)</t>
+  </si>
+  <si>
+    <t>48.0%/53.8%</t>
+  </si>
+  <si>
+    <t>42.6%/47.8%</t>
+  </si>
+  <si>
+    <t>48%/53.7%</t>
+  </si>
+  <si>
+    <t>46.9%/52.5%</t>
+  </si>
+  <si>
+    <t>48%/53.8%</t>
+  </si>
+  <si>
+    <t>Results of beamsearch on test dataset(gta&amp;cityscape)</t>
+  </si>
+  <si>
+    <t>(0, 2, 9, 13)-53.764%</t>
+  </si>
+  <si>
+    <t>(0,13)-56.794%</t>
   </si>
 </sst>
 </file>
@@ -494,7 +651,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +661,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,10 +971,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -820,16 +983,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -841,10 +1004,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -865,28 +1028,28 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -895,19 +1058,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -919,38 +1079,41 @@
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -963,41 +1126,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1352,8 +1521,8 @@
   <sheetPr/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1431,7 +1600,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="6">
         <v>0.232</v>
       </c>
       <c r="G3" s="2"/>
@@ -1456,7 +1625,7 @@
       <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>0.233</v>
       </c>
       <c r="G4" s="2"/>
@@ -1479,7 +1648,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="14">
+      <c r="F5" s="8">
         <v>0.237</v>
       </c>
       <c r="G5" s="2"/>
@@ -1499,8 +1668,8 @@
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="10">
+      <c r="E6" s="9"/>
+      <c r="F6" s="15">
         <v>0.261</v>
       </c>
       <c r="G6" s="2"/>
@@ -1523,7 +1692,7 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="15">
         <v>0.279</v>
       </c>
       <c r="G7" s="2"/>
@@ -1546,7 +1715,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>0.217</v>
       </c>
       <c r="G8" s="2"/>
@@ -1569,22 +1738,22 @@
         <v>15</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>0.321</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>0.309</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="4">
         <v>0.296</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1602,7 +1771,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>0.354</v>
       </c>
       <c r="G10" s="2"/>
@@ -1616,6 +1785,198 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="6" width="16.625" customWidth="1"/>
+    <col min="7" max="8" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.477</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.534</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.538</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:8">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:8">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="5:8">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="5:8">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1962,7 +2323,7 @@
       <c r="C16">
         <v>36</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="17">
         <v>75.6</v>
       </c>
       <c r="E16">
@@ -2039,22 +2400,22 @@
       <c r="B3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>0.142</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>0.138</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>0.126</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>0.142</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>0.123</v>
       </c>
     </row>
@@ -2063,20 +2424,20 @@
         <v>100</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>0.272</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="10">
+      <c r="E4" s="14"/>
+      <c r="F4" s="15">
         <v>0.298</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="6">
         <v>0.265</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>0.292</v>
       </c>
     </row>
@@ -2085,20 +2446,20 @@
         <v>200</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="10">
+      <c r="C5" s="15">
         <v>0.322</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>0.291</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="12">
+      <c r="E5" s="14"/>
+      <c r="F5" s="16">
         <v>0.297</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="6">
         <v>0.276</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <v>0.296</v>
       </c>
     </row>
@@ -2107,20 +2468,20 @@
         <v>400</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>0.321</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>0.31</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9">
+      <c r="E6" s="14"/>
+      <c r="F6" s="6">
         <v>0.296</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="6">
         <v>0.286</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="6">
         <v>0.295</v>
       </c>
     </row>
@@ -2129,11 +2490,11 @@
         <v>600</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>0.315</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="G7" s="9">
+      <c r="E7" s="14"/>
+      <c r="G7" s="6">
         <v>0.29</v>
       </c>
     </row>
@@ -2142,11 +2503,11 @@
         <v>800</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>0.317</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="G8" s="9">
+      <c r="E8" s="14"/>
+      <c r="G8" s="6">
         <v>0.292</v>
       </c>
     </row>
@@ -2167,7 +2528,7 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E8"/>
     </sheetView>
   </sheetViews>
@@ -2221,52 +2582,52 @@
       <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:8">
       <c r="A4" s="2">
         <v>100</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>0.284</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:8">
       <c r="A5" s="2">
         <v>200</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="10">
+      <c r="C5" s="15">
         <v>0.286</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:8">
       <c r="A6" s="2">
         <v>400</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:8">
       <c r="A7" s="2">
@@ -2274,10 +2635,10 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="14"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:8">
@@ -2286,10 +2647,10 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="2"/>
     </row>
   </sheetData>
@@ -2309,7 +2670,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A1" sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
@@ -2359,7 +2720,7 @@
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2376,7 +2737,7 @@
       <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="13">
         <v>0.266</v>
       </c>
     </row>
@@ -2393,7 +2754,7 @@
       <c r="D5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="13">
         <v>0.27</v>
       </c>
     </row>
@@ -2407,7 +2768,7 @@
       <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="13">
         <v>0.266</v>
       </c>
     </row>
@@ -2421,7 +2782,7 @@
       <c r="D7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="13">
         <v>0.286</v>
       </c>
     </row>
@@ -2440,7 +2801,7 @@
   <sheetPr/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -2494,10 +2855,10 @@
       <c r="D3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="13">
         <v>0.248</v>
       </c>
     </row>
@@ -2514,10 +2875,10 @@
       <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="13">
         <v>0.238</v>
       </c>
     </row>
@@ -2534,10 +2895,10 @@
       <c r="D5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="13">
         <v>0.26</v>
       </c>
     </row>
@@ -2554,10 +2915,10 @@
       <c r="D6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="13">
         <v>0.248</v>
       </c>
     </row>
@@ -2574,10 +2935,10 @@
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="13">
         <v>0.305</v>
       </c>
     </row>
@@ -2594,10 +2955,10 @@
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="13">
         <v>0.287</v>
       </c>
     </row>
@@ -2608,4 +2969,812 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="16.125" customWidth="1"/>
+    <col min="11" max="11" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.491</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.551</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="4">
+        <v>0.487</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.545</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.446</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4">
+        <v>0.441</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.491</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:11">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="8">
+        <v>0.437</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.493</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:11">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:11">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:11">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.442</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.491</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:9">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="1:9">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" ht="30" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="16.125" customWidth="1"/>
+    <col min="11" max="11" width="18.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.548</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="12">
+        <v>0.491</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.444</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.497</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.492</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:11">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="8">
+        <v>0.442</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.495</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4">
+        <v>0.439</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.491</v>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:11">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.387</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.433</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:11">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4">
+        <v>0.427</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.478</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="4">
+        <v>0.424</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.475</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:11">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="10">
+        <v>0.457</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.511</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.433</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.485</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0.458</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0.513</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:11">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4">
+        <v>0.469</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.525</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="13">
+        <v>0.469</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0.525</v>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:9">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="1:9">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" ht="30" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="24.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="45" customHeight="1" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A4" s="2">
+        <v>100</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A5" s="2">
+        <v>200</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A6" s="2">
+        <v>400</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A7" s="2">
+        <v>600</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A8" s="2">
+        <v>800</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" customFormat="1" ht="30" customHeight="1" spans="1:3">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1"/>
+    <row r="11" ht="30" customHeight="1"/>
+    <row r="12" ht="30" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="E3:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sample gta dataset, modify evaluation
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="8010" firstSheet="6" activeTab="6"/>
+    <workbookView windowWidth="19815" windowHeight="8010" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,16 +15,17 @@
     <sheet name="mutual normalization" sheetId="5" r:id="rId6"/>
     <sheet name="Test on gta" sheetId="7" r:id="rId7"/>
     <sheet name="Test on gta (fix data)" sheetId="9" r:id="rId8"/>
-    <sheet name="facr on SCOT (gta)" sheetId="10" r:id="rId9"/>
-    <sheet name="gta beamsearch(on test)" sheetId="8" r:id="rId10"/>
-    <sheet name="Sheet3" sheetId="11" r:id="rId11"/>
+    <sheet name="Test on gta (uniformly sampled)" sheetId="11" r:id="rId9"/>
+    <sheet name="facr on SCOT (gta)" sheetId="10" r:id="rId10"/>
+    <sheet name="facr on SCOT (gta) (uni sample)" sheetId="12" r:id="rId11"/>
+    <sheet name="gta beamsearch(on val)" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="154">
   <si>
     <t>Backbones we have</t>
   </si>
@@ -426,7 +427,46 @@
     <t>gta denormalization</t>
   </si>
   <si>
-    <t>PCK for SCOT with default resnet50 pretrained on ImageNet(Supervised,for classification) as the backbone(hyperfeature_id = 0, 2, 9, 13),without CAM</t>
+    <t>Test results on gta&amp;cityscape datasets(the first 500 images in cityscape and uniformaly sample on gta(1 every 4 images)) of different backbones</t>
+  </si>
+  <si>
+    <t>Acc[gta,cs]</t>
+  </si>
+  <si>
+    <t>Acc(with Mutual Normalization)</t>
+  </si>
+  <si>
+    <t>Normalized Acc(with Mutual Normalization)</t>
+  </si>
+  <si>
+    <t>(50.3%,47.1%)</t>
+  </si>
+  <si>
+    <t>(55.9%,48.9%)</t>
+  </si>
+  <si>
+    <t>(50.5%,47.7%)</t>
+  </si>
+  <si>
+    <t>(56.1%.49.5%)</t>
+  </si>
+  <si>
+    <t>(49.8%,47.0%)</t>
+  </si>
+  <si>
+    <t>(55.4%,48.7%)</t>
+  </si>
+  <si>
+    <t>(3,13)--layer1,layer3</t>
+  </si>
+  <si>
+    <t>45.6%/45.1%</t>
+  </si>
+  <si>
+    <t>50.7%/50.1%</t>
+  </si>
+  <si>
+    <t>ACC/Normalized ACC for SCOT with default resnet50 pretrained on ImageNet(Supervised,for classification) as the backbone(hyperfeature_id = 0, 2, 9, 13),without CAM</t>
   </si>
   <si>
     <t>Acc and Normalized Acc(without factorization)</t>
@@ -465,13 +505,148 @@
     <t>48%/53.8%</t>
   </si>
   <si>
-    <t>Results of beamsearch on test dataset(gta&amp;cityscape)</t>
-  </si>
-  <si>
-    <t>(0, 2, 9, 13)-53.764%</t>
-  </si>
-  <si>
-    <t>(0,13)-56.794%</t>
+    <t>ACC/Normalized ACC for SCOT with default resnet50 pretrained on ImageNet(Supervised,for classification) as the backbone(hyperfeature_id = 0, 11, 12, 13),without CAM</t>
+  </si>
+  <si>
+    <t>Acc and Normalized Acc(reconstruction with SVD),(gta,cs)</t>
+  </si>
+  <si>
+    <t>(50.5%,47.7%)/(56.1%.49.5%)</t>
+  </si>
+  <si>
+    <t>(46.5%,44.4%)/(51.8%,46.1%)</t>
+  </si>
+  <si>
+    <t>(52.1%,48.1%)/(57.9%,49.9%)</t>
+  </si>
+  <si>
+    <t>ACC/Normalized ACC for SCOT with default resnet50 pretrained on ImageNet(Supervised,for classification) as the backbone(optimal hyperfeature_id = 0, 2, 9, 13),without CAM</t>
+  </si>
+  <si>
+    <t>(51.8%,47.6%)/(57.7%,49.3%)</t>
+  </si>
+  <si>
+    <t>47.0%/52.3%</t>
+  </si>
+  <si>
+    <t>43.5%/48.4%</t>
+  </si>
+  <si>
+    <t>51.8%/57.6%</t>
+  </si>
+  <si>
+    <t>46.6%/51.9%</t>
+  </si>
+  <si>
+    <t>43.6%/48.6%</t>
+  </si>
+  <si>
+    <t>46.7%/52.1%</t>
+  </si>
+  <si>
+    <t>51.7%/57.5%</t>
+  </si>
+  <si>
+    <t>51.1%/56.9%</t>
+  </si>
+  <si>
+    <t>51.7%/57.6%</t>
+  </si>
+  <si>
+    <t>51.3%/57.1%</t>
+  </si>
+  <si>
+    <t>52.0%/57.9%</t>
+  </si>
+  <si>
+    <t>51.6%/57.5%</t>
+  </si>
+  <si>
+    <t>52.0%/57.8%</t>
+  </si>
+  <si>
+    <t>51.8%/57.7%</t>
+  </si>
+  <si>
+    <t>51.9%/57.8%</t>
+  </si>
+  <si>
+    <t>52.1%/58.0%</t>
+  </si>
+  <si>
+    <t>ACC/Normalized ACC for SCOT with default resnet50 pretrained on ImageNet(Simsiam,self-supervised) as the backbone(optimal hyperfeature_id = 0,13),without CAM</t>
+  </si>
+  <si>
+    <t>54.4%/60.6%</t>
+  </si>
+  <si>
+    <t>49.5%/55.1%</t>
+  </si>
+  <si>
+    <t>43.7%/48.7%</t>
+  </si>
+  <si>
+    <t>53.3%/59.3%</t>
+  </si>
+  <si>
+    <t>47.0%/52.4%</t>
+  </si>
+  <si>
+    <t>42.6%/47.4%</t>
+  </si>
+  <si>
+    <t>45.7%/50.8%</t>
+  </si>
+  <si>
+    <t>53.3%/59.4%</t>
+  </si>
+  <si>
+    <t>53.9%/60.0%</t>
+  </si>
+  <si>
+    <t>53.6%/59.7%</t>
+  </si>
+  <si>
+    <t>52.5%/58.4%</t>
+  </si>
+  <si>
+    <t>53.8%/59.9%</t>
+  </si>
+  <si>
+    <t>54.1%/60.2%</t>
+  </si>
+  <si>
+    <t>52.8%/58.8%</t>
+  </si>
+  <si>
+    <t>53.7%/59.8%</t>
+  </si>
+  <si>
+    <t>54.1%/60.3%</t>
+  </si>
+  <si>
+    <t>53.0%/59.0%</t>
+  </si>
+  <si>
+    <t>ACC/Normalized ACC for SCOT with default resnet50 pretrained on ImageNet(Simsiam,self-supervised) as the backbone(hyperfeature_id = 0,11,12,13),without CAM</t>
+  </si>
+  <si>
+    <t>53.4%/59.4%</t>
+  </si>
+  <si>
+    <t>Results of beamsearch on val set(gta&amp;cityscape)</t>
+  </si>
+  <si>
+    <t>results on test set</t>
+  </si>
+  <si>
+    <t>hyperfeats_id--(nor acc)</t>
+  </si>
+  <si>
+    <t>(0, 2, 9, 13)-54.946%</t>
+  </si>
+  <si>
+    <t>(0,13)-57.925%</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1288,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1130,6 +1305,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1144,23 +1322,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1521,7 +1702,7 @@
   <sheetPr/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1600,7 +1781,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>0.232</v>
       </c>
       <c r="G3" s="2"/>
@@ -1648,7 +1829,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="8">
+      <c r="F5" s="9">
         <v>0.237</v>
       </c>
       <c r="G5" s="2"/>
@@ -1668,8 +1849,8 @@
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="15">
+      <c r="E6" s="10"/>
+      <c r="F6" s="11">
         <v>0.261</v>
       </c>
       <c r="G6" s="2"/>
@@ -1692,7 +1873,7 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="11">
         <v>0.279</v>
       </c>
       <c r="G7" s="2"/>
@@ -1741,19 +1922,19 @@
       <c r="F9" s="4">
         <v>0.321</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="20" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="4">
         <v>0.309</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="4">
         <v>0.296</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="20" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1792,10 +1973,872 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="24.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="45" customHeight="1" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A4" s="2">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A5" s="2">
+        <v>200</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A6" s="2">
+        <v>400</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A7" s="2">
+        <v>600</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A8" s="2">
+        <v>800</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" customFormat="1" ht="30" customHeight="1" spans="1:3">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1"/>
+    <row r="11" ht="30" customHeight="1"/>
+    <row r="12" ht="30" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="E3:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="28.75" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="29.25" customWidth="1"/>
+    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="24.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="45" customHeight="1" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A4" s="2">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A5" s="2">
+        <v>200</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A6" s="2">
+        <v>400</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A7" s="2">
+        <v>600</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A8" s="2">
+        <v>800</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="30" customHeight="1"/>
+    <row r="11" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" s="5" customFormat="1" ht="60" customHeight="1" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A16" s="2">
+        <v>100</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A17" s="2">
+        <v>200</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A18" s="2">
+        <v>400</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A19" s="2">
+        <v>600</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A20" s="2">
+        <v>800</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" s="5" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A21" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="23" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A27" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" s="5" customFormat="1" ht="49" customHeight="1" spans="1:8">
+      <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A30" s="2">
+        <v>100</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A31" s="2">
+        <v>200</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A32" s="2">
+        <v>400</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A33" s="2">
+        <v>600</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" s="5" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A34" s="2">
+        <v>800</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" s="5" customFormat="1" ht="30" customHeight="1" spans="1:5">
+      <c r="A35" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="39" ht="30" customHeight="1" spans="1:8">
+      <c r="A39" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" ht="48" customHeight="1" spans="1:8">
+      <c r="A40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" ht="30" customHeight="1" spans="1:8">
+      <c r="A41" s="2">
+        <v>4</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" ht="30" customHeight="1" spans="1:8">
+      <c r="A42" s="2">
+        <v>100</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" ht="30" customHeight="1" spans="1:8">
+      <c r="A43" s="2">
+        <v>200</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" ht="30" customHeight="1" spans="1:8">
+      <c r="A44" s="2">
+        <v>400</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" ht="30" customHeight="1" spans="1:8">
+      <c r="A45" s="2">
+        <v>600</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" ht="30" customHeight="1" spans="1:8">
+      <c r="A46" s="2">
+        <v>800</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" ht="30" customHeight="1" spans="1:8">
+      <c r="A47" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="E3:E9"/>
+    <mergeCell ref="E15:E21"/>
+    <mergeCell ref="E29:E35"/>
+    <mergeCell ref="E41:E47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1808,15 +2851,19 @@
     <col min="7" max="8" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:6">
+    <row r="1" ht="30" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:8">
       <c r="A2" s="2" t="s">
@@ -1829,7 +2876,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>65</v>
@@ -1855,20 +2902,12 @@
         <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.477</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.534</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.48</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.538</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:8">
       <c r="A4" s="2" t="s">
@@ -1881,12 +2920,16 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="4">
+        <v>0.544</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.606</v>
+      </c>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:8">
       <c r="A5" s="2" t="s">
@@ -1957,26 +3000,12 @@
       <c r="H10" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2323,7 +3352,7 @@
       <c r="C16">
         <v>36</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="19">
         <v>75.6</v>
       </c>
       <c r="E16">
@@ -2347,7 +3376,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -2356,16 +3385,16 @@
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
       <c r="A2" s="2" t="s">
@@ -2397,7 +3426,7 @@
       <c r="A3" s="2">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="4">
@@ -2406,7 +3435,7 @@
       <c r="D3" s="4">
         <v>0.138</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="17" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="4">
@@ -2423,21 +3452,21 @@
       <c r="A4" s="2">
         <v>100</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>0.272</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15">
+      <c r="E4" s="17"/>
+      <c r="F4" s="11">
         <v>0.298</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>0.265</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <v>0.292</v>
       </c>
     </row>
@@ -2445,21 +3474,21 @@
       <c r="A5" s="2">
         <v>200</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="15">
+      <c r="B5" s="6"/>
+      <c r="C5" s="11">
         <v>0.322</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>0.291</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="16">
+      <c r="E5" s="17"/>
+      <c r="F5" s="18">
         <v>0.297</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>0.276</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="7">
         <v>0.296</v>
       </c>
     </row>
@@ -2467,21 +3496,21 @@
       <c r="A6" s="2">
         <v>400</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4">
         <v>0.321</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="7">
         <v>0.31</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="6">
+      <c r="E6" s="17"/>
+      <c r="F6" s="7">
         <v>0.296</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>0.286</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="7">
         <v>0.295</v>
       </c>
     </row>
@@ -2489,12 +3518,12 @@
       <c r="A7" s="2">
         <v>600</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="D7" s="6">
+      <c r="B7" s="6"/>
+      <c r="D7" s="7">
         <v>0.315</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="G7" s="6">
+      <c r="E7" s="17"/>
+      <c r="G7" s="7">
         <v>0.29</v>
       </c>
     </row>
@@ -2502,12 +3531,12 @@
       <c r="A8" s="2">
         <v>800</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="D8" s="6">
+      <c r="B8" s="6"/>
+      <c r="D8" s="7">
         <v>0.317</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="G8" s="6">
+      <c r="E8" s="17"/>
+      <c r="G8" s="7">
         <v>0.292</v>
       </c>
     </row>
@@ -2538,16 +3567,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" ht="30" customHeight="1" spans="1:8">
       <c r="A2" s="2" t="s">
@@ -2579,12 +3608,12 @@
       <c r="A3" s="2">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="14"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -2593,64 +3622,64 @@
       <c r="A4" s="2">
         <v>100</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7">
         <v>0.284</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" ht="30" customHeight="1" spans="1:8">
       <c r="A5" s="2">
         <v>200</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="15">
+      <c r="B5" s="6"/>
+      <c r="C5" s="11">
         <v>0.286</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" ht="30" customHeight="1" spans="1:8">
       <c r="A6" s="2">
         <v>400</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" ht="30" customHeight="1" spans="1:8">
       <c r="A7" s="2">
         <v>600</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="14"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:8">
       <c r="A8" s="2">
         <v>800</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="14"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="2"/>
     </row>
   </sheetData>
@@ -2660,6 +3689,7 @@
     <mergeCell ref="E3:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2670,7 +3700,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
@@ -2720,7 +3750,7 @@
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2737,7 +3767,7 @@
       <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="15">
         <v>0.266</v>
       </c>
     </row>
@@ -2754,7 +3784,7 @@
       <c r="D5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="15">
         <v>0.27</v>
       </c>
     </row>
@@ -2768,7 +3798,7 @@
       <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="15">
         <v>0.266</v>
       </c>
     </row>
@@ -2782,7 +3812,7 @@
       <c r="D7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="15">
         <v>0.286</v>
       </c>
     </row>
@@ -2792,6 +3822,7 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2855,10 +3886,10 @@
       <c r="D3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="15">
         <v>0.248</v>
       </c>
     </row>
@@ -2875,10 +3906,10 @@
       <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="15">
         <v>0.238</v>
       </c>
     </row>
@@ -2895,10 +3926,10 @@
       <c r="D5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="15">
         <v>0.26</v>
       </c>
     </row>
@@ -2915,10 +3946,10 @@
       <c r="D6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="15">
         <v>0.248</v>
       </c>
     </row>
@@ -2935,10 +3966,10 @@
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="15">
         <v>0.305</v>
       </c>
     </row>
@@ -2955,10 +3986,10 @@
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="15">
         <v>0.287</v>
       </c>
     </row>
@@ -2967,6 +3998,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2976,7 +4008,7 @@
   <sheetPr/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -3037,10 +4069,10 @@
       <c r="I2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="13" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3060,7 +4092,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>0.491</v>
       </c>
       <c r="G3" s="4">
@@ -3120,7 +4152,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="8">
+      <c r="F5" s="9">
         <v>0.437</v>
       </c>
       <c r="G5" s="4">
@@ -3142,8 +4174,8 @@
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -3164,7 +4196,7 @@
       <c r="E7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -3210,10 +4242,10 @@
         <v>15</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="12" t="s">
         <v>75</v>
       </c>
       <c r="H9" s="4">
@@ -3225,7 +4257,7 @@
       <c r="J9" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="7" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3276,6 +4308,7 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -3285,7 +4318,7 @@
   <sheetPr/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -3346,10 +4379,10 @@
       <c r="I2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="13" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3369,7 +4402,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>0.49</v>
       </c>
       <c r="G3" s="4">
@@ -3377,10 +4410,10 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="12">
+      <c r="J3" s="16">
         <v>0.491</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="16">
         <v>0.55</v>
       </c>
     </row>
@@ -3429,7 +4462,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="8">
+      <c r="F5" s="9">
         <v>0.442</v>
       </c>
       <c r="G5" s="4">
@@ -3455,8 +4488,8 @@
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -3477,7 +4510,7 @@
       <c r="E7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <v>0.387</v>
       </c>
       <c r="G7" s="4">
@@ -3531,10 +4564,10 @@
         <v>15</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="10">
+      <c r="F9" s="12">
         <v>0.457</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="12">
         <v>0.511</v>
       </c>
       <c r="H9" s="4">
@@ -3543,10 +4576,10 @@
       <c r="I9" s="4">
         <v>0.485</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="16">
         <v>0.458</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="16">
         <v>0.513</v>
       </c>
     </row>
@@ -3572,10 +4605,10 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="13">
+      <c r="J10" s="15">
         <v>0.469</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="15">
         <v>0.525</v>
       </c>
     </row>
@@ -3607,6 +4640,7 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -3614,166 +4648,408 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="18.625" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="28.75" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="18.625" customWidth="1"/>
-    <col min="6" max="6" width="24.25" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="20.25" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="16.125" customWidth="1"/>
+    <col min="11" max="11" width="18.25" customWidth="1"/>
+    <col min="12" max="13" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="30" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" s="2" customFormat="1" ht="45" customHeight="1" spans="1:8">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" ht="30" customHeight="1" spans="1:13">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H3" s="4">
+        <v>0.472</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.526</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K3" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A3" s="2">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="M3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A4" s="2">
-        <v>100</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.532</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.592</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="7">
+        <v>0.534</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.594</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.512</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.498</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.554</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="7">
+        <v>0.495</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0.55</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.494</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.549</v>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="9">
+        <v>0.501</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.557</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="7">
+        <v>0.498</v>
+      </c>
+      <c r="K6" s="15">
+        <v>0.554</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0.499</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.555</v>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="7">
+        <v>0.47</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.523</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" ht="30" customHeight="1" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.421</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.468</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A5" s="2">
-        <v>200</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="30" customHeight="1" spans="1:8">
-      <c r="A6" s="2">
-        <v>400</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
-      <c r="A7" s="2">
-        <v>600</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" s="2" customFormat="1" ht="30" customHeight="1" spans="1:7">
-      <c r="A8" s="2">
-        <v>800</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" customFormat="1" ht="30" customHeight="1" spans="1:3">
-      <c r="A9">
-        <v>1000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" ht="30" customHeight="1"/>
-    <row r="11" ht="30" customHeight="1"/>
-    <row r="12" ht="30" customHeight="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="7">
+        <v>0.478</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.532</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="12" ht="30" customHeight="1" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4">
+        <v>0.517</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.576</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="J12" s="4">
+        <v>0.519</v>
+      </c>
+      <c r="K12" s="15">
+        <v>0.578</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.511</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.569</v>
+      </c>
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="1:13">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" ht="30" customHeight="1" spans="1:13">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" ht="30" customHeight="1" spans="12:13">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="E3:E8"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>

</xml_diff>